<commit_message>
version 3.4.6: scaling behavior (configs & excel)
</commit_message>
<xml_diff>
--- a/datasets/sgt_files/InVitroBioFilm_SGT_scaling.xlsx
+++ b/datasets/sgt_files/InVitroBioFilm_SGT_scaling.xlsx
@@ -7,12 +7,12 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Nodes-Number of edg." sheetId="1" r:id="rId1"/>
-    <sheet name="Nodes-Number of edg. (Fit Data)" sheetId="2" r:id="rId2"/>
+    <sheet name="Nodes-Number of edge." sheetId="1" r:id="rId1"/>
+    <sheet name="Nodes-Number of edge. (Fitting)" sheetId="2" r:id="rId2"/>
     <sheet name="Nodes-Average degree" sheetId="3" r:id="rId3"/>
-    <sheet name="Nodes-Average degree (Fit Data)" sheetId="4" r:id="rId4"/>
+    <sheet name="Nodes-Average degree (Fitting)" sheetId="4" r:id="rId4"/>
     <sheet name="Nodes-Graph density" sheetId="5" r:id="rId5"/>
-    <sheet name="Nodes-Graph density (Fit Data)" sheetId="6" r:id="rId6"/>
+    <sheet name="Nodes-Graph density (Fitting)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>

<commit_message>
version 3.4.8: kernel-size vs nodes plot
</commit_message>
<xml_diff>
--- a/datasets/sgt_files/InVitroBioFilm_SGT_scaling.xlsx
+++ b/datasets/sgt_files/InVitroBioFilm_SGT_scaling.xlsx
@@ -19,7 +19,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+  <si>
+    <t>kernel-dim</t>
+  </si>
   <si>
     <t>x-avg</t>
   </si>
@@ -403,13 +406,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,258 +434,294 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
-        <v>11.9</v>
+        <v>62</v>
       </c>
       <c r="B2">
-        <v>1.345362404707371</v>
+        <v>12.1</v>
       </c>
       <c r="C2">
-        <v>8.6</v>
+        <v>1.12989675044522</v>
       </c>
       <c r="D2">
-        <v>1.284090685617215</v>
+        <v>0.113967</v>
       </c>
       <c r="E2">
-        <v>1.075546961392531</v>
+        <v>0.0111726845525644</v>
       </c>
       <c r="F2">
-        <v>0.9344984512435677</v>
+        <v>1.08278537031645</v>
       </c>
       <c r="G2">
-        <v>0.9402403879769228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>-0.9432208836866045</v>
+      </c>
+      <c r="H2">
+        <v>-0.928579184308906</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
-        <v>37.7</v>
+        <v>125</v>
       </c>
       <c r="B3">
-        <v>1.633333333333333</v>
+        <v>39.5</v>
       </c>
       <c r="C3">
-        <v>29</v>
+        <v>1.796601730428249</v>
       </c>
       <c r="D3">
-        <v>2.144761058952722</v>
+        <v>0.039636</v>
       </c>
       <c r="E3">
-        <v>1.576341350205793</v>
+        <v>0.002826119915675514</v>
       </c>
       <c r="F3">
-        <v>1.462397997898956</v>
+        <v>1.59659709562646</v>
       </c>
       <c r="G3">
-        <v>1.46664151410671</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>-1.401910180260961</v>
+      </c>
+      <c r="H3">
+        <v>-1.410745692789158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
-        <v>78.8</v>
+        <v>188</v>
       </c>
       <c r="B4">
-        <v>2.731706833139716</v>
+        <v>80.09999999999999</v>
       </c>
       <c r="C4">
-        <v>61.3</v>
+        <v>3.572891763761611</v>
       </c>
       <c r="D4">
-        <v>5.901129835322498</v>
+        <v>0.019578</v>
       </c>
       <c r="E4">
-        <v>1.896526217489555</v>
+        <v>0.001783419810987369</v>
       </c>
       <c r="F4">
-        <v>1.787460474518415</v>
+        <v>1.903632516084238</v>
       </c>
       <c r="G4">
-        <v>1.803198149869531</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>-1.708231675828481</v>
+      </c>
+      <c r="H4">
+        <v>-1.698871069010518</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
-        <v>125.4</v>
+        <v>251</v>
       </c>
       <c r="B5">
-        <v>1.528979325490629</v>
+        <v>137.2</v>
       </c>
       <c r="C5">
-        <v>111.1</v>
+        <v>4.304519588628781</v>
       </c>
       <c r="D5">
-        <v>4.269920634183054</v>
+        <v>0.012534</v>
       </c>
       <c r="E5">
-        <v>2.098297536494698</v>
+        <v>0.0009046155721262668</v>
       </c>
       <c r="F5">
-        <v>2.045714058940868</v>
+        <v>2.137354111370733</v>
       </c>
       <c r="G5">
-        <v>2.015286487753453</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>-1.901910309636048</v>
+      </c>
+      <c r="H5">
+        <v>-1.918197954724794</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
-        <v>204.4</v>
+        <v>314</v>
       </c>
       <c r="B6">
-        <v>4.13440846232364</v>
+        <v>203.4</v>
       </c>
       <c r="C6">
-        <v>183.2</v>
+        <v>4.77772609791171</v>
       </c>
       <c r="D6">
-        <v>5.801915392542554</v>
+        <v>0.008934000000000001</v>
       </c>
       <c r="E6">
-        <v>2.310480891462675</v>
+        <v>0.000431483745026649</v>
       </c>
       <c r="F6">
-        <v>2.262925469331832</v>
+        <v>2.308350948586726</v>
       </c>
       <c r="G6">
-        <v>2.238319252289456</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>-2.04895405186418</v>
+      </c>
+      <c r="H6">
+        <v>-2.07866324560903</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
-        <v>290.6</v>
+        <v>376</v>
       </c>
       <c r="B7">
-        <v>4.487513540679045</v>
+        <v>290.4</v>
       </c>
       <c r="C7">
-        <v>230.3</v>
+        <v>4.742713709821976</v>
       </c>
       <c r="D7">
-        <v>7.449161026585477</v>
+        <v>0.005514</v>
       </c>
       <c r="E7">
-        <v>2.463295609962003</v>
+        <v>0.0003042593922589372</v>
       </c>
       <c r="F7">
-        <v>2.362293937964231</v>
+        <v>2.462996612028056</v>
       </c>
       <c r="G7">
-        <v>2.398947729173705</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>-2.258533238230245</v>
+      </c>
+      <c r="H7">
+        <v>-2.22378441727581</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
-        <v>389.3</v>
+        <v>439</v>
       </c>
       <c r="B8">
-        <v>4.887739763939974</v>
+        <v>397.9</v>
       </c>
       <c r="C8">
-        <v>330.3</v>
+        <v>4.958606435055898</v>
       </c>
       <c r="D8">
-        <v>12.88672874618604</v>
+        <v>0.004329999999999999</v>
       </c>
       <c r="E8">
-        <v>2.590284403718162</v>
+        <v>0.0001732114956410868</v>
       </c>
       <c r="F8">
-        <v>2.518908573691414</v>
+        <v>2.599773939146388</v>
       </c>
       <c r="G8">
-        <v>2.532429744013196</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>-2.363512103646635</v>
+      </c>
+      <c r="H8">
+        <v>-2.352137747897287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
-        <v>518.1</v>
+        <v>502</v>
       </c>
       <c r="B9">
-        <v>6.563281699475246</v>
+        <v>515.9</v>
       </c>
       <c r="C9">
-        <v>420.3</v>
+        <v>5.700779673771728</v>
       </c>
       <c r="D9">
-        <v>11.81246987062589</v>
+        <v>0.003257</v>
       </c>
       <c r="E9">
-        <v>2.714413592287121</v>
+        <v>0.0001395711686241507</v>
       </c>
       <c r="F9">
-        <v>2.623559390005437</v>
+        <v>2.712565527873308</v>
       </c>
       <c r="G9">
-        <v>2.662905935655674</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>-2.487182241435127</v>
+      </c>
+      <c r="H9">
+        <v>-2.457982600872541</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
-        <v>658.6</v>
+        <v>565</v>
       </c>
       <c r="B10">
-        <v>9.318082778483278</v>
+        <v>667</v>
       </c>
       <c r="C10">
-        <v>562.6</v>
+        <v>4.695151163109069</v>
       </c>
       <c r="D10">
-        <v>12.02331069215131</v>
+        <v>0.002504999999999999</v>
       </c>
       <c r="E10">
-        <v>2.818621726375889</v>
+        <v>7.528095524249295E-05</v>
       </c>
       <c r="F10">
-        <v>2.750199727829182</v>
+        <v>2.824125833916549</v>
       </c>
       <c r="G10">
-        <v>2.772442464741398</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>-2.601192269796736</v>
+      </c>
+      <c r="H10">
+        <v>-2.56267200479263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
-        <v>817</v>
+        <v>628</v>
       </c>
       <c r="B11">
-        <v>8.299933065325822</v>
+        <v>811.5</v>
       </c>
       <c r="C11">
-        <v>701.1</v>
+        <v>8.364275886836296</v>
       </c>
       <c r="D11">
-        <v>11.38463877336475</v>
+        <v>0.002171</v>
       </c>
       <c r="E11">
-        <v>2.912222056532416</v>
+        <v>6.04510821518799E-05</v>
       </c>
       <c r="F11">
-        <v>2.84577996711189</v>
+        <v>2.909288524162251</v>
       </c>
       <c r="G11">
-        <v>2.87082878915145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>-2.66334017654558</v>
+      </c>
+      <c r="H11">
+        <v>-2.642589599089996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
+        <v>638</v>
+      </c>
+      <c r="B12">
         <v>496</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0</v>
       </c>
-      <c r="C12">
-        <v>563</v>
-      </c>
       <c r="D12">
-        <v>0</v>
+        <v>0.004589999999999999</v>
       </c>
       <c r="E12">
+        <v>2.891205793294678E-19</v>
+      </c>
+      <c r="F12">
         <v>2.695481676490198</v>
       </c>
-      <c r="F12">
-        <v>2.750508394851346</v>
-      </c>
       <c r="G12">
-        <v>2.643005988655647</v>
+        <v>-2.338187314462739</v>
+      </c>
+      <c r="H12">
+        <v>-2.441950929022662</v>
       </c>
     </row>
   </sheetData>
@@ -700,810 +739,810 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>11.9</v>
+        <v>12.1</v>
       </c>
       <c r="B2">
-        <v>11.53329490015203</v>
+        <v>0.114118894657337</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>20.03232323232323</v>
+        <v>20.17474747474747</v>
       </c>
       <c r="B3">
-        <v>19.17535974889559</v>
+        <v>0.07153840198621657</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>28.16464646464647</v>
+        <v>28.24949494949495</v>
       </c>
       <c r="B4">
-        <v>26.74160821203446</v>
+        <v>0.05259964516128546</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>36.2969696969697</v>
+        <v>36.32424242424242</v>
       </c>
       <c r="B5">
-        <v>34.25517998973264</v>
+        <v>0.04180625295572488</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>44.42929292929293</v>
+        <v>44.3989898989899</v>
       </c>
       <c r="B6">
-        <v>41.72836626881682</v>
+        <v>0.03480208572938091</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>52.56161616161616</v>
+        <v>52.47373737373737</v>
       </c>
       <c r="B7">
-        <v>49.16881501243679</v>
+        <v>0.02987537705570119</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>60.6939393939394</v>
+        <v>60.54848484848484</v>
       </c>
       <c r="B8">
-        <v>56.58174841161382</v>
+        <v>0.02621373526820083</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>68.82626262626263</v>
+        <v>68.62323232323232</v>
       </c>
       <c r="B9">
-        <v>63.97095969599865</v>
+        <v>0.02338103360402072</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>76.95858585858586</v>
+        <v>76.69797979797978</v>
       </c>
       <c r="B10">
-        <v>71.33932896396621</v>
+        <v>0.02112174936903392</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>85.09090909090909</v>
+        <v>84.77272727272725</v>
       </c>
       <c r="B11">
-        <v>78.68911724290442</v>
+        <v>0.01927604335909764</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>93.22323232323232</v>
+        <v>92.84747474747473</v>
       </c>
       <c r="B12">
-        <v>86.02214649100083</v>
+        <v>0.01773870091217781</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>101.3555555555556</v>
+        <v>100.9222222222222</v>
       </c>
       <c r="B13">
-        <v>93.33991598258662</v>
+        <v>0.01643757540808223</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>109.4878787878788</v>
+        <v>108.9969696969697</v>
       </c>
       <c r="B14">
-        <v>100.6436809089506</v>
+        <v>0.01532150915408134</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>117.620202020202</v>
+        <v>117.0717171717172</v>
       </c>
       <c r="B15">
-        <v>107.93450737939</v>
+        <v>0.01435319723341663</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>125.7525252525253</v>
+        <v>125.1464646464646</v>
       </c>
       <c r="B16">
-        <v>115.2133120614473</v>
+        <v>0.0135047825124472</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>133.8848484848485</v>
+        <v>133.2212121212121</v>
       </c>
       <c r="B17">
-        <v>122.4808914723075</v>
+        <v>0.01275503402534345</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>142.0171717171717</v>
+        <v>141.2959595959596</v>
       </c>
       <c r="B18">
-        <v>129.737944090963</v>
+        <v>0.01208748145851442</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>150.149494949495</v>
+        <v>149.3707070707071</v>
       </c>
       <c r="B19">
-        <v>136.9850873630349</v>
+        <v>0.01148914749613198</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>158.2818181818182</v>
+        <v>157.4454545454545</v>
       </c>
       <c r="B20">
-        <v>144.2228709918053</v>
+        <v>0.01094966553484734</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>166.4141414141414</v>
+        <v>165.520202020202</v>
       </c>
       <c r="B21">
-        <v>151.4517874763915</v>
+        <v>0.01046065249826879</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>174.5464646464646</v>
+        <v>173.5949494949495</v>
       </c>
       <c r="B22">
-        <v>158.6722805743542</v>
+        <v>0.01001525453838841</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>182.6787878787879</v>
+        <v>181.6696969696969</v>
       </c>
       <c r="B23">
-        <v>165.8847521754888</v>
+        <v>0.009607812388484292</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>190.8111111111111</v>
+        <v>189.7444444444444</v>
       </c>
       <c r="B24">
-        <v>173.0895679427375</v>
+        <v>0.009233611095551531</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>198.9434343434343</v>
+        <v>197.8191919191919</v>
       </c>
       <c r="B25">
-        <v>180.2870619846039</v>
+        <v>0.008888690275485224</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>207.0757575757576</v>
+        <v>205.8939393939393</v>
       </c>
       <c r="B26">
-        <v>187.4775407582362</v>
+        <v>0.00856969845168928</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>215.2080808080808</v>
+        <v>213.9686868686868</v>
       </c>
       <c r="B27">
-        <v>194.6612863551547</v>
+        <v>0.008273779955781664</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>223.3404040404041</v>
+        <v>222.0434343434343</v>
       </c>
       <c r="B28">
-        <v>201.8385592869551</v>
+        <v>0.007998486190224757</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>231.4727272727273</v>
+        <v>230.1181818181818</v>
       </c>
       <c r="B29">
-        <v>209.0096008625501</v>
+        <v>0.007741705333417221</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>239.6050505050505</v>
+        <v>238.1929292929293</v>
       </c>
       <c r="B30">
-        <v>216.1746352291121</v>
+        <v>0.007501606158254927</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>247.7373737373737</v>
+        <v>246.2676767676767</v>
       </c>
       <c r="B31">
-        <v>223.3338711341068</v>
+        <v>0.007276592760105602</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>255.869696969697</v>
+        <v>254.3424242424242</v>
       </c>
       <c r="B32">
-        <v>230.4875034544522</v>
+        <v>0.007065267796277352</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>264.0020202020202</v>
+        <v>262.4171717171717</v>
       </c>
       <c r="B33">
-        <v>237.6357145300106</v>
+        <v>0.006866402423782412</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>272.1343434343434</v>
+        <v>270.4919191919192</v>
       </c>
       <c r="B34">
-        <v>244.7786753317172</v>
+        <v>0.006678911551119365</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>280.2666666666667</v>
+        <v>278.5666666666667</v>
       </c>
       <c r="B35">
-        <v>251.9165464891828</v>
+        <v>0.006501833337750171</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>288.3989898989899</v>
+        <v>286.6414141414141</v>
       </c>
       <c r="B36">
-        <v>259.0494791982699</v>
+        <v>0.006334312112962199</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>296.5313131313131</v>
+        <v>294.7161616161616</v>
       </c>
       <c r="B37">
-        <v>266.1776160256525</v>
+        <v>0.006175584065620148</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>304.6636363636363</v>
+        <v>302.7909090909091</v>
       </c>
       <c r="B38">
-        <v>273.3010916245614</v>
+        <v>0.006024965193333106</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>312.7959595959596</v>
+        <v>310.8656565656565</v>
       </c>
       <c r="B39">
-        <v>280.4200333736278</v>
+        <v>0.005881841104820782</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>320.9282828282828</v>
+        <v>318.940404040404</v>
       </c>
       <c r="B40">
-        <v>287.5345619488772</v>
+        <v>0.005745658350741072</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>329.060606060606</v>
+        <v>327.0151515151515</v>
       </c>
       <c r="B41">
-        <v>294.6447918373839</v>
+        <v>0.005615917021766245</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>337.1929292929293</v>
+        <v>335.089898989899</v>
       </c>
       <c r="B42">
-        <v>301.7508317998337</v>
+        <v>0.005492164402560705</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>345.3252525252525</v>
+        <v>343.1646464646465</v>
       </c>
       <c r="B43">
-        <v>308.8527852881869</v>
+        <v>0.005373989509709177</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>353.4575757575757</v>
+        <v>351.2393939393939</v>
       </c>
       <c r="B44">
-        <v>315.9507508237555</v>
+        <v>0.005261018372958773</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>361.589898989899</v>
+        <v>359.3141414141414</v>
       </c>
       <c r="B45">
-        <v>323.044822340271</v>
+        <v>0.005152909944174143</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>369.7222222222222</v>
+        <v>367.3888888888889</v>
       </c>
       <c r="B46">
-        <v>330.1350894959003</v>
+        <v>0.005049352538531013</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>377.8545454545454</v>
+        <v>375.4636363636363</v>
       </c>
       <c r="B47">
-        <v>337.2216379576412</v>
+        <v>0.004950060728737752</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>385.9868686868687</v>
+        <v>383.5383838383838</v>
       </c>
       <c r="B48">
-        <v>344.3045496610847</v>
+        <v>0.004854772626283929</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>394.1191919191919</v>
+        <v>391.6131313131313</v>
       </c>
       <c r="B49">
-        <v>351.3839030481529</v>
+        <v>0.004763247494494139</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>402.2515151515152</v>
+        <v>399.6878787878787</v>
       </c>
       <c r="B50">
-        <v>358.4597732850949</v>
+        <v>0.004675263647001852</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>410.3838383838383</v>
+        <v>407.7626262626262</v>
       </c>
       <c r="B51">
-        <v>365.5322324627465</v>
+        <v>0.004590616592533375</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>418.5161616161616</v>
+        <v>415.8373737373737</v>
       </c>
       <c r="B52">
-        <v>372.6013497808208</v>
+        <v>0.004509117392907075</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
-        <v>426.6484848484848</v>
+        <v>423.9121212121212</v>
       </c>
       <c r="B53">
-        <v>379.667191717787</v>
+        <v>0.004430591206145848</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54">
-        <v>434.7808080808081</v>
+        <v>431.9868686868687</v>
       </c>
       <c r="B54">
-        <v>386.7298221877192</v>
+        <v>0.004354875990761184</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55">
-        <v>442.9131313131313</v>
+        <v>440.0616161616161</v>
       </c>
       <c r="B55">
-        <v>393.7893026853394</v>
+        <v>0.004281821350746441</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56">
-        <v>451.0454545454545</v>
+        <v>448.1363636363636</v>
       </c>
       <c r="B56">
-        <v>400.8456924203433</v>
+        <v>0.004211287503737038</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <v>459.1777777777777</v>
+        <v>456.2111111111111</v>
       </c>
       <c r="B57">
-        <v>407.8990484419801</v>
+        <v>0.00414314435725427</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <v>467.310101010101</v>
+        <v>464.2858585858585</v>
       </c>
       <c r="B58">
-        <v>414.9494257547545</v>
+        <v>0.00407727068002698</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <v>475.4424242424242</v>
+        <v>472.360606060606</v>
       </c>
       <c r="B59">
-        <v>421.9968774260248</v>
+        <v>0.004013553357146009</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <v>483.5747474747474</v>
+        <v>480.4353535353535</v>
       </c>
       <c r="B60">
-        <v>429.0414546861965</v>
+        <v>0.003951886719303136</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <v>491.7070707070707</v>
+        <v>488.510101010101</v>
       </c>
       <c r="B61">
-        <v>436.0832070221346</v>
+        <v>0.003892171937642248</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>499.8393939393939</v>
+        <v>496.5848484848485</v>
       </c>
       <c r="B62">
-        <v>443.1221822643595</v>
+        <v>0.003834316476841483</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>507.9717171717172</v>
+        <v>504.6595959595959</v>
       </c>
       <c r="B63">
-        <v>450.158426668534</v>
+        <v>0.003778233599980349</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>516.1040404040403</v>
+        <v>512.7343434343434</v>
       </c>
       <c r="B64">
-        <v>457.1919849917008</v>
+        <v>0.003723841919549707</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>524.2363636363636</v>
+        <v>520.8090909090909</v>
       </c>
       <c r="B65">
-        <v>464.2229005636867</v>
+        <v>0.003671064989655256</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>532.3686868686868</v>
+        <v>528.8838383838383</v>
       </c>
       <c r="B66">
-        <v>471.2512153540482</v>
+        <v>0.003619830935063521</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>540.50101010101</v>
+        <v>536.9585858585858</v>
       </c>
       <c r="B67">
-        <v>478.2769700349036</v>
+        <v>0.003570072113257467</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>548.6333333333333</v>
+        <v>545.0333333333333</v>
       </c>
       <c r="B68">
-        <v>485.3002040399605</v>
+        <v>0.003521724806118537</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>556.7656565656565</v>
+        <v>553.1080808080808</v>
       </c>
       <c r="B69">
-        <v>492.3209556200219</v>
+        <v>0.003474728938243024</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>564.8979797979798</v>
+        <v>561.1828282828283</v>
       </c>
       <c r="B70">
-        <v>499.3392618952312</v>
+        <v>0.003429027819241569</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>573.030303030303</v>
+        <v>569.2575757575758</v>
       </c>
       <c r="B71">
-        <v>506.3551589042891</v>
+        <v>0.003384567907668399</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>581.1626262626262</v>
+        <v>577.3323232323232</v>
       </c>
       <c r="B72">
-        <v>513.3686816508622</v>
+        <v>0.003341298594487549</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>589.2949494949495</v>
+        <v>585.4070707070706</v>
       </c>
       <c r="B73">
-        <v>520.3798641473762</v>
+        <v>0.00329917200421184</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>597.4272727272727</v>
+        <v>593.4818181818181</v>
       </c>
       <c r="B74">
-        <v>527.3887394563787</v>
+        <v>0.003258142812051314</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>605.559595959596</v>
+        <v>601.5565656565656</v>
       </c>
       <c r="B75">
-        <v>534.3953397296362</v>
+        <v>0.003218168075584502</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>613.6919191919192</v>
+        <v>609.631313131313</v>
       </c>
       <c r="B76">
-        <v>541.3996962451176</v>
+        <v>0.003179207079621927</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>621.8242424242424</v>
+        <v>617.7060606060605</v>
       </c>
       <c r="B77">
-        <v>548.401839442007</v>
+        <v>0.003141221193068869</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>629.9565656565657</v>
+        <v>625.780808080808</v>
       </c>
       <c r="B78">
-        <v>555.4017989538729</v>
+        <v>0.003104173736716384</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>638.0888888888888</v>
+        <v>633.8555555555555</v>
       </c>
       <c r="B79">
-        <v>562.3996036401149</v>
+        <v>0.003068029860997553</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>646.221212121212</v>
+        <v>641.930303030303</v>
       </c>
       <c r="B80">
-        <v>569.3952816157978</v>
+        <v>0.003032756432841862</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <v>654.3535353535353</v>
+        <v>650.0050505050505</v>
       </c>
       <c r="B81">
-        <v>576.3888602799744</v>
+        <v>0.002998321930845916</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82">
-        <v>662.4858585858585</v>
+        <v>658.0797979797979</v>
       </c>
       <c r="B82">
-        <v>583.3803663425931</v>
+        <v>0.002964696348054624</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <v>670.6181818181818</v>
+        <v>666.1545454545454</v>
       </c>
       <c r="B83">
-        <v>590.3698258500751</v>
+        <v>0.002931851101714743</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <v>678.750505050505</v>
+        <v>674.2292929292929</v>
       </c>
       <c r="B84">
-        <v>597.3572642096444</v>
+        <v>0.002899758949423204</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>686.8828282828282</v>
+        <v>682.3040404040404</v>
       </c>
       <c r="B85">
-        <v>604.3427062124849</v>
+        <v>0.002868393911146696</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <v>695.0151515151515</v>
+        <v>690.3787878787878</v>
       </c>
       <c r="B86">
-        <v>611.3261760557937</v>
+        <v>0.002837731196637552</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <v>703.1474747474747</v>
+        <v>698.4535353535352</v>
       </c>
       <c r="B87">
-        <v>618.3076973637967</v>
+        <v>0.002807747137814382</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <v>711.279797979798</v>
+        <v>706.5282828282827</v>
       </c>
       <c r="B88">
-        <v>625.2872932077858</v>
+        <v>0.002778419125714995</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>719.4121212121212</v>
+        <v>714.6030303030302</v>
       </c>
       <c r="B89">
-        <v>632.2649861252343</v>
+        <v>0.002749725551664224</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <v>727.5444444444444</v>
+        <v>722.6777777777777</v>
       </c>
       <c r="B90">
-        <v>639.2407981380436</v>
+        <v>0.002721645752330935</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>735.6767676767677</v>
+        <v>730.7525252525252</v>
       </c>
       <c r="B91">
-        <v>646.2147507699681</v>
+        <v>0.00269415995837694</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
-        <v>743.8090909090909</v>
+        <v>738.8272727272727</v>
       </c>
       <c r="B92">
-        <v>653.1868650632653</v>
+        <v>0.002667249246426297</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>751.9414141414142</v>
+        <v>746.9020202020201</v>
       </c>
       <c r="B93">
-        <v>660.1571615946145</v>
+        <v>0.00264089549410671</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>760.0737373737373</v>
+        <v>754.9767676767676</v>
       </c>
       <c r="B94">
-        <v>667.125660490341</v>
+        <v>0.002615081337935753</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>768.2060606060605</v>
+        <v>763.0515151515151</v>
       </c>
       <c r="B95">
-        <v>674.0923814409869</v>
+        <v>0.002589790133843706</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>776.3383838383838</v>
+        <v>771.1262626262626</v>
       </c>
       <c r="B96">
-        <v>681.057343715259</v>
+        <v>0.002565005920142038</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <v>784.470707070707</v>
+        <v>779.2010101010101</v>
       </c>
       <c r="B97">
-        <v>688.0205661733909</v>
+        <v>0.002540713382762229</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>792.6030303030303</v>
+        <v>787.2757575757574</v>
       </c>
       <c r="B98">
-        <v>694.9820672799465</v>
+        <v>0.002516897822603894</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <v>800.7353535353535</v>
+        <v>795.3505050505049</v>
       </c>
       <c r="B99">
-        <v>701.9418651160945</v>
+        <v>0.002493545124844073</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
-        <v>808.8676767676767</v>
+        <v>803.4252525252524</v>
       </c>
       <c r="B100">
-        <v>708.8999773913837</v>
+        <v>0.002470641730071381</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101">
-        <v>817</v>
+        <v>811.5</v>
       </c>
       <c r="B101">
-        <v>715.8564214550388</v>
+        <v>0.002448174607119392</v>
       </c>
     </row>
   </sheetData>
@@ -1513,13 +1552,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1541,258 +1580,294 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
-        <v>11.9</v>
+        <v>62</v>
       </c>
       <c r="B2">
-        <v>1.345362404707371</v>
+        <v>12.1</v>
       </c>
       <c r="C2">
-        <v>1.410798</v>
+        <v>1.12989675044522</v>
       </c>
       <c r="D2">
-        <v>0.1262844054487946</v>
+        <v>0.113967</v>
       </c>
       <c r="E2">
-        <v>1.075546961392531</v>
+        <v>0.0111726845525644</v>
       </c>
       <c r="F2">
-        <v>0.1494648353237909</v>
+        <v>1.08278537031645</v>
       </c>
       <c r="G2">
-        <v>0.1587913879138593</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>-0.9432208836866045</v>
+      </c>
+      <c r="H2">
+        <v>-0.928579184308906</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
-        <v>37.7</v>
+        <v>125</v>
       </c>
       <c r="B3">
-        <v>1.633333333333333</v>
+        <v>39.5</v>
       </c>
       <c r="C3">
-        <v>1.533037</v>
+        <v>1.796601730428249</v>
       </c>
       <c r="D3">
-        <v>0.08404640928346936</v>
+        <v>0.039636</v>
       </c>
       <c r="E3">
-        <v>1.576341350205793</v>
+        <v>0.002826119915675514</v>
       </c>
       <c r="F3">
-        <v>0.1855526367212484</v>
+        <v>1.59659709562646</v>
       </c>
       <c r="G3">
-        <v>0.1870105216986532</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>-1.401910180260961</v>
+      </c>
+      <c r="H3">
+        <v>-1.410745692789158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
-        <v>78.8</v>
+        <v>188</v>
       </c>
       <c r="B4">
-        <v>2.731706833139716</v>
+        <v>80.09999999999999</v>
       </c>
       <c r="C4">
-        <v>1.545694</v>
+        <v>3.572891763761611</v>
       </c>
       <c r="D4">
-        <v>0.1167062390620142</v>
+        <v>0.019578</v>
       </c>
       <c r="E4">
-        <v>1.896526217489555</v>
+        <v>0.001783419810987369</v>
       </c>
       <c r="F4">
-        <v>0.1891235211055446</v>
+        <v>1.903632516084238</v>
       </c>
       <c r="G4">
-        <v>0.2050525361612315</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>-1.708231675828481</v>
+      </c>
+      <c r="H4">
+        <v>-1.698871069010518</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
-        <v>125.4</v>
+        <v>251</v>
       </c>
       <c r="B5">
-        <v>1.528979325490629</v>
+        <v>137.2</v>
       </c>
       <c r="C5">
-        <v>1.772188</v>
+        <v>4.304519588628781</v>
       </c>
       <c r="D5">
-        <v>0.06372116163061967</v>
+        <v>0.012534</v>
       </c>
       <c r="E5">
-        <v>2.098297536494698</v>
+        <v>0.0009046155721262668</v>
       </c>
       <c r="F5">
-        <v>0.2485097914966998</v>
+        <v>2.137354111370733</v>
       </c>
       <c r="G5">
-        <v>0.2164220961485811</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>-1.901910309636048</v>
+      </c>
+      <c r="H5">
+        <v>-1.918197954724794</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
-        <v>204.4</v>
+        <v>314</v>
       </c>
       <c r="B6">
-        <v>4.13440846232364</v>
+        <v>203.4</v>
       </c>
       <c r="C6">
-        <v>1.801775</v>
+        <v>4.77772609791171</v>
       </c>
       <c r="D6">
-        <v>0.07252252764562961</v>
+        <v>0.008934000000000001</v>
       </c>
       <c r="E6">
-        <v>2.310480891462675</v>
+        <v>0.000431483745026649</v>
       </c>
       <c r="F6">
-        <v>0.2557005566988577</v>
+        <v>2.308350948586726</v>
       </c>
       <c r="G6">
-        <v>0.2283783612635652</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>-2.04895405186418</v>
+      </c>
+      <c r="H6">
+        <v>-2.07866324560903</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
-        <v>290.6</v>
+        <v>376</v>
       </c>
       <c r="B7">
-        <v>4.487513540679045</v>
+        <v>290.4</v>
       </c>
       <c r="C7">
-        <v>1.588418</v>
+        <v>4.742713709821976</v>
       </c>
       <c r="D7">
-        <v>0.05741524245548583</v>
+        <v>0.005514</v>
       </c>
       <c r="E7">
-        <v>2.463295609962003</v>
+        <v>0.0003042593922589372</v>
       </c>
       <c r="F7">
-        <v>0.2009647998577111</v>
+        <v>2.462996612028056</v>
       </c>
       <c r="G7">
-        <v>0.2369892784023075</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>-2.258533238230245</v>
+      </c>
+      <c r="H7">
+        <v>-2.22378441727581</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
-        <v>389.3</v>
+        <v>439</v>
       </c>
       <c r="B8">
-        <v>4.887739763939974</v>
+        <v>397.9</v>
       </c>
       <c r="C8">
-        <v>1.70431</v>
+        <v>4.958606435055898</v>
       </c>
       <c r="D8">
-        <v>0.082260099562303</v>
+        <v>0.004329999999999999</v>
       </c>
       <c r="E8">
-        <v>2.590284403718162</v>
+        <v>0.0001732114956410868</v>
       </c>
       <c r="F8">
-        <v>0.2315485922173505</v>
+        <v>2.599773939146388</v>
       </c>
       <c r="G8">
-        <v>0.2441449371721004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>-2.363512103646635</v>
+      </c>
+      <c r="H8">
+        <v>-2.352137747897287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
-        <v>518.1</v>
+        <v>502</v>
       </c>
       <c r="B9">
-        <v>6.563281699475246</v>
+        <v>515.9</v>
       </c>
       <c r="C9">
-        <v>1.626741</v>
+        <v>5.700779673771728</v>
       </c>
       <c r="D9">
-        <v>0.0578871389755771</v>
+        <v>0.003257</v>
       </c>
       <c r="E9">
-        <v>2.714413592287121</v>
+        <v>0.0001395711686241507</v>
       </c>
       <c r="F9">
-        <v>0.2113184126635239</v>
+        <v>2.712565527873308</v>
       </c>
       <c r="G9">
-        <v>0.2511394607871233</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>-2.487182241435127</v>
+      </c>
+      <c r="H9">
+        <v>-2.457982600872541</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
-        <v>658.6</v>
+        <v>565</v>
       </c>
       <c r="B10">
-        <v>9.318082778483278</v>
+        <v>667</v>
       </c>
       <c r="C10">
-        <v>1.713368</v>
+        <v>4.695151163109069</v>
       </c>
       <c r="D10">
-        <v>0.05174093665775892</v>
+        <v>0.002504999999999999</v>
       </c>
       <c r="E10">
-        <v>2.818621726375889</v>
+        <v>7.528095524249295E-05</v>
       </c>
       <c r="F10">
-        <v>0.2338506514680618</v>
+        <v>2.824125833916549</v>
       </c>
       <c r="G10">
-        <v>0.2570114580438882</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>-2.601192269796736</v>
+      </c>
+      <c r="H10">
+        <v>-2.56267200479263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
-        <v>817</v>
+        <v>628</v>
       </c>
       <c r="B11">
-        <v>8.299933065325822</v>
+        <v>811.5</v>
       </c>
       <c r="C11">
-        <v>1.718732</v>
+        <v>8.364275886836296</v>
       </c>
       <c r="D11">
-        <v>0.03766979629476232</v>
+        <v>0.002171</v>
       </c>
       <c r="E11">
-        <v>2.912222056532416</v>
+        <v>6.04510821518799E-05</v>
       </c>
       <c r="F11">
-        <v>0.2352081629028564</v>
+        <v>2.909288524162251</v>
       </c>
       <c r="G11">
-        <v>0.2622857188942285</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>-2.66334017654558</v>
+      </c>
+      <c r="H11">
+        <v>-2.642589599089996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
+        <v>638</v>
+      </c>
+      <c r="B12">
         <v>496</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0</v>
       </c>
-      <c r="C12">
-        <v>2.27016</v>
-      </c>
       <c r="D12">
-        <v>0</v>
+        <v>0.004589999999999999</v>
       </c>
       <c r="E12">
+        <v>2.891205793294678E-19</v>
+      </c>
+      <c r="F12">
         <v>2.695481676490198</v>
       </c>
-      <c r="F12">
-        <v>0.3560564671791732</v>
-      </c>
       <c r="G12">
-        <v>0.2500726711492806</v>
+        <v>-2.338187314462739</v>
+      </c>
+      <c r="H12">
+        <v>-2.441950929022662</v>
       </c>
     </row>
   </sheetData>
@@ -1810,810 +1885,810 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>11.9</v>
+        <v>12.1</v>
       </c>
       <c r="B2">
-        <v>1.447575165001846</v>
+        <v>0.114118894657337</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>20.03232323232323</v>
+        <v>20.17474747474747</v>
       </c>
       <c r="B3">
-        <v>1.490793527168109</v>
+        <v>0.07153840198621657</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>28.16464646464647</v>
+        <v>28.24949494949495</v>
       </c>
       <c r="B4">
-        <v>1.519763403641782</v>
+        <v>0.05259964516128546</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>36.2969696969697</v>
+        <v>36.32424242424242</v>
       </c>
       <c r="B5">
-        <v>1.541696490065472</v>
+        <v>0.04180625295572488</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>44.42929292929293</v>
+        <v>44.3989898989899</v>
       </c>
       <c r="B6">
-        <v>1.559402939079937</v>
+        <v>0.03480208572938091</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>52.56161616161616</v>
+        <v>52.47373737373737</v>
       </c>
       <c r="B7">
-        <v>1.574279455032929</v>
+        <v>0.02987537705570119</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>60.6939393939394</v>
+        <v>60.54848484848484</v>
       </c>
       <c r="B8">
-        <v>1.587124210256446</v>
+        <v>0.02621373526820083</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>68.82626262626263</v>
+        <v>68.62323232323232</v>
       </c>
       <c r="B9">
-        <v>1.598437216937782</v>
+        <v>0.02338103360402072</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>76.95858585858586</v>
+        <v>76.69797979797978</v>
       </c>
       <c r="B10">
-        <v>1.608552885202207</v>
+        <v>0.02112174936903392</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>85.09090909090909</v>
+        <v>84.77272727272725</v>
       </c>
       <c r="B11">
-        <v>1.617706129944206</v>
+        <v>0.01927604335909764</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>93.22323232323232</v>
+        <v>92.84747474747473</v>
       </c>
       <c r="B12">
-        <v>1.626068415622183</v>
+        <v>0.01773870091217781</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>101.3555555555556</v>
+        <v>100.9222222222222</v>
       </c>
       <c r="B13">
-        <v>1.633768799655381</v>
+        <v>0.01643757540808223</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>109.4878787878788</v>
+        <v>108.9969696969697</v>
       </c>
       <c r="B14">
-        <v>1.640906901483526</v>
+        <v>0.01532150915408134</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>117.620202020202</v>
+        <v>117.0717171717172</v>
       </c>
       <c r="B15">
-        <v>1.647561255375935</v>
+        <v>0.01435319723341663</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>125.7525252525253</v>
+        <v>125.1464646464646</v>
       </c>
       <c r="B16">
-        <v>1.653794890527843</v>
+        <v>0.0135047825124472</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>133.8848484848485</v>
+        <v>133.2212121212121</v>
       </c>
       <c r="B17">
-        <v>1.659659175755748</v>
+        <v>0.01275503402534345</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>142.0171717171717</v>
+        <v>141.2959595959596</v>
       </c>
       <c r="B18">
-        <v>1.665196539454405</v>
+        <v>0.01208748145851442</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>150.149494949495</v>
+        <v>149.3707070707071</v>
       </c>
       <c r="B19">
-        <v>1.670442438408028</v>
+        <v>0.01148914749613198</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>158.2818181818182</v>
+        <v>157.4454545454545</v>
       </c>
       <c r="B20">
-        <v>1.675426811716933</v>
+        <v>0.01094966553484734</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>166.4141414141414</v>
+        <v>165.520202020202</v>
       </c>
       <c r="B21">
-        <v>1.68017517363069</v>
+        <v>0.01046065249826879</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>174.5464646464646</v>
+        <v>173.5949494949495</v>
       </c>
       <c r="B22">
-        <v>1.684709447971873</v>
+        <v>0.01001525453838841</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>182.6787878787879</v>
+        <v>181.6696969696969</v>
       </c>
       <c r="B23">
-        <v>1.689048614272976</v>
+        <v>0.009607812388484292</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>190.8111111111111</v>
+        <v>189.7444444444444</v>
       </c>
       <c r="B24">
-        <v>1.693209214485977</v>
+        <v>0.009233611095551531</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>198.9434343434343</v>
+        <v>197.8191919191919</v>
       </c>
       <c r="B25">
-        <v>1.697205754929482</v>
+        <v>0.008888690275485224</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>207.0757575757576</v>
+        <v>205.8939393939393</v>
       </c>
       <c r="B26">
-        <v>1.701051028472715</v>
+        <v>0.00856969845168928</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>215.2080808080808</v>
+        <v>213.9686868686868</v>
       </c>
       <c r="B27">
-        <v>1.704756375254502</v>
+        <v>0.008273779955781664</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>223.3404040404041</v>
+        <v>222.0434343434343</v>
       </c>
       <c r="B28">
-        <v>1.708331895513118</v>
+        <v>0.007998486190224757</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>231.4727272727273</v>
+        <v>230.1181818181818</v>
       </c>
       <c r="B29">
-        <v>1.711786624724964</v>
+        <v>0.007741705333417221</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>239.6050505050505</v>
+        <v>238.1929292929293</v>
       </c>
       <c r="B30">
-        <v>1.715128678800505</v>
+        <v>0.007501606158254927</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>247.7373737373737</v>
+        <v>246.2676767676767</v>
       </c>
       <c r="B31">
-        <v>1.718365375287039</v>
+        <v>0.007276592760105602</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>255.869696969697</v>
+        <v>254.3424242424242</v>
       </c>
       <c r="B32">
-        <v>1.721503335191358</v>
+        <v>0.007065267796277352</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>264.0020202020202</v>
+        <v>262.4171717171717</v>
       </c>
       <c r="B33">
-        <v>1.724548569031556</v>
+        <v>0.006866402423782412</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>272.1343434343434</v>
+        <v>270.4919191919192</v>
       </c>
       <c r="B34">
-        <v>1.727506549965815</v>
+        <v>0.006678911551119365</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>280.2666666666667</v>
+        <v>278.5666666666667</v>
       </c>
       <c r="B35">
-        <v>1.730382276262853</v>
+        <v>0.006501833337750171</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>288.3989898989899</v>
+        <v>286.6414141414141</v>
       </c>
       <c r="B36">
-        <v>1.733180324928357</v>
+        <v>0.006334312112962199</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>296.5313131313131</v>
+        <v>294.7161616161616</v>
       </c>
       <c r="B37">
-        <v>1.735904897950914</v>
+        <v>0.006175584065620148</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>304.6636363636363</v>
+        <v>302.7909090909091</v>
       </c>
       <c r="B38">
-        <v>1.738559862355677</v>
+        <v>0.006024965193333106</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>312.7959595959596</v>
+        <v>310.8656565656565</v>
       </c>
       <c r="B39">
-        <v>1.741148785036396</v>
+        <v>0.005881841104820782</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>320.9282828282828</v>
+        <v>318.940404040404</v>
       </c>
       <c r="B40">
-        <v>1.743674963163253</v>
+        <v>0.005745658350741072</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>329.060606060606</v>
+        <v>327.0151515151515</v>
       </c>
       <c r="B41">
-        <v>1.74614145082523</v>
+        <v>0.005615917021766245</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>337.1929292929293</v>
+        <v>335.089898989899</v>
       </c>
       <c r="B42">
-        <v>1.748551082453944</v>
+        <v>0.005492164402560705</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>345.3252525252525</v>
+        <v>343.1646464646465</v>
       </c>
       <c r="B43">
-        <v>1.750906493485291</v>
+        <v>0.005373989509709177</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>353.4575757575757</v>
+        <v>351.2393939393939</v>
       </c>
       <c r="B44">
-        <v>1.753210138641397</v>
+        <v>0.005261018372958773</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>361.589898989899</v>
+        <v>359.3141414141414</v>
       </c>
       <c r="B45">
-        <v>1.755464308154924</v>
+        <v>0.005152909944174143</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>369.7222222222222</v>
+        <v>367.3888888888889</v>
       </c>
       <c r="B46">
-        <v>1.757671142207975</v>
+        <v>0.005049352538531013</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>377.8545454545454</v>
+        <v>375.4636363636363</v>
       </c>
       <c r="B47">
-        <v>1.759832643816672</v>
+        <v>0.004950060728737752</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>385.9868686868687</v>
+        <v>383.5383838383838</v>
       </c>
       <c r="B48">
-        <v>1.761950690358316</v>
+        <v>0.004854772626283929</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>394.1191919191919</v>
+        <v>391.6131313131313</v>
       </c>
       <c r="B49">
-        <v>1.76402704390946</v>
+        <v>0.004763247494494139</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>402.2515151515152</v>
+        <v>399.6878787878787</v>
       </c>
       <c r="B50">
-        <v>1.766063360539379</v>
+        <v>0.004675263647001852</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>410.3838383838383</v>
+        <v>407.7626262626262</v>
       </c>
       <c r="B51">
-        <v>1.768061198683288</v>
+        <v>0.004590616592533375</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>418.5161616161616</v>
+        <v>415.8373737373737</v>
       </c>
       <c r="B52">
-        <v>1.770022026702724</v>
+        <v>0.004509117392907075</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
-        <v>426.6484848484848</v>
+        <v>423.9121212121212</v>
       </c>
       <c r="B53">
-        <v>1.771947229726139</v>
+        <v>0.004430591206145848</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54">
-        <v>434.7808080808081</v>
+        <v>431.9868686868687</v>
       </c>
       <c r="B54">
-        <v>1.773838115850526</v>
+        <v>0.004354875990761184</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55">
-        <v>442.9131313131313</v>
+        <v>440.0616161616161</v>
       </c>
       <c r="B55">
-        <v>1.775695921774533</v>
+        <v>0.004281821350746441</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56">
-        <v>451.0454545454545</v>
+        <v>448.1363636363636</v>
       </c>
       <c r="B56">
-        <v>1.777521817924554</v>
+        <v>0.004211287503737038</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <v>459.1777777777777</v>
+        <v>456.2111111111111</v>
       </c>
       <c r="B57">
-        <v>1.77931691312771</v>
+        <v>0.00414314435725427</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <v>467.310101010101</v>
+        <v>464.2858585858585</v>
       </c>
       <c r="B58">
-        <v>1.781082258879015</v>
+        <v>0.00407727068002698</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <v>475.4424242424242</v>
+        <v>472.360606060606</v>
       </c>
       <c r="B59">
-        <v>1.782818853244374</v>
+        <v>0.004013553357146009</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <v>483.5747474747474</v>
+        <v>480.4353535353535</v>
       </c>
       <c r="B60">
-        <v>1.784527644436137</v>
+        <v>0.003951886719303136</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <v>491.7070707070707</v>
+        <v>488.510101010101</v>
       </c>
       <c r="B61">
-        <v>1.786209534093701</v>
+        <v>0.003892171937642248</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>499.8393939393939</v>
+        <v>496.5848484848485</v>
       </c>
       <c r="B62">
-        <v>1.787865380297924</v>
+        <v>0.003834316476841483</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>507.9717171717172</v>
+        <v>504.6595959595959</v>
       </c>
       <c r="B63">
-        <v>1.78949600034489</v>
+        <v>0.003778233599980349</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>516.1040404040403</v>
+        <v>512.7343434343434</v>
       </c>
       <c r="B64">
-        <v>1.791102173301784</v>
+        <v>0.003723841919549707</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>524.2363636363636</v>
+        <v>520.8090909090909</v>
       </c>
       <c r="B65">
-        <v>1.792684642365106</v>
+        <v>0.003671064989655256</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>532.3686868686868</v>
+        <v>528.8838383838383</v>
       </c>
       <c r="B66">
-        <v>1.794244117039331</v>
+        <v>0.003619830935063521</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>540.50101010101</v>
+        <v>536.9585858585858</v>
       </c>
       <c r="B67">
-        <v>1.795781275152209</v>
+        <v>0.003570072113257467</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>548.6333333333333</v>
+        <v>545.0333333333333</v>
       </c>
       <c r="B68">
-        <v>1.797296764721203</v>
+        <v>0.003521724806118537</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>556.7656565656565</v>
+        <v>553.1080808080808</v>
       </c>
       <c r="B69">
-        <v>1.798791205684091</v>
+        <v>0.003474728938243024</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>564.8979797979798</v>
+        <v>561.1828282828283</v>
       </c>
       <c r="B70">
-        <v>1.80026519150545</v>
+        <v>0.003429027819241569</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>573.030303030303</v>
+        <v>569.2575757575758</v>
       </c>
       <c r="B71">
-        <v>1.801719290669572</v>
+        <v>0.003384567907668399</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>581.1626262626262</v>
+        <v>577.3323232323232</v>
       </c>
       <c r="B72">
-        <v>1.80315404806932</v>
+        <v>0.003341298594487549</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>589.2949494949495</v>
+        <v>585.4070707070706</v>
       </c>
       <c r="B73">
-        <v>1.804569986299538</v>
+        <v>0.00329917200421184</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>597.4272727272727</v>
+        <v>593.4818181818181</v>
       </c>
       <c r="B74">
-        <v>1.805967606862778</v>
+        <v>0.003258142812051314</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>605.559595959596</v>
+        <v>601.5565656565656</v>
       </c>
       <c r="B75">
-        <v>1.8073473912944</v>
+        <v>0.003218168075584502</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>613.6919191919192</v>
+        <v>609.631313131313</v>
       </c>
       <c r="B76">
-        <v>1.808709802213449</v>
+        <v>0.003179207079621927</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>621.8242424242424</v>
+        <v>617.7060606060605</v>
       </c>
       <c r="B77">
-        <v>1.810055284305105</v>
+        <v>0.003141221193068869</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>629.9565656565657</v>
+        <v>625.780808080808</v>
       </c>
       <c r="B78">
-        <v>1.81138426524</v>
+        <v>0.003104173736716384</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>638.0888888888888</v>
+        <v>633.8555555555555</v>
       </c>
       <c r="B79">
-        <v>1.812697156535217</v>
+        <v>0.003068029860997553</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>646.221212121212</v>
+        <v>641.930303030303</v>
       </c>
       <c r="B80">
-        <v>1.813994354361367</v>
+        <v>0.003032756432841862</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <v>654.3535353535353</v>
+        <v>650.0050505050505</v>
       </c>
       <c r="B81">
-        <v>1.815276240299737</v>
+        <v>0.002998321930845916</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82">
-        <v>662.4858585858585</v>
+        <v>658.0797979797979</v>
       </c>
       <c r="B82">
-        <v>1.816543182053199</v>
+        <v>0.002964696348054624</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <v>670.6181818181818</v>
+        <v>666.1545454545454</v>
       </c>
       <c r="B83">
-        <v>1.817795534114222</v>
+        <v>0.002931851101714743</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <v>678.750505050505</v>
+        <v>674.2292929292929</v>
       </c>
       <c r="B84">
-        <v>1.819033638393051</v>
+        <v>0.002899758949423204</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>686.8828282828282</v>
+        <v>682.3040404040404</v>
       </c>
       <c r="B85">
-        <v>1.820257824808903</v>
+        <v>0.002868393911146696</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <v>695.0151515151515</v>
+        <v>690.3787878787878</v>
       </c>
       <c r="B86">
-        <v>1.821468411846737</v>
+        <v>0.002837731196637552</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <v>703.1474747474747</v>
+        <v>698.4535353535352</v>
       </c>
       <c r="B87">
-        <v>1.822665707081997</v>
+        <v>0.002807747137814382</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <v>711.279797979798</v>
+        <v>706.5282828282827</v>
       </c>
       <c r="B88">
-        <v>1.82385000767552</v>
+        <v>0.002778419125714995</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>719.4121212121212</v>
+        <v>714.6030303030302</v>
       </c>
       <c r="B89">
-        <v>1.825021600840604</v>
+        <v>0.002749725551664224</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <v>727.5444444444444</v>
+        <v>722.6777777777777</v>
       </c>
       <c r="B90">
-        <v>1.826180764284133</v>
+        <v>0.002721645752330935</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>735.6767676767677</v>
+        <v>730.7525252525252</v>
       </c>
       <c r="B91">
-        <v>1.827327766623431</v>
+        <v>0.00269415995837694</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
-        <v>743.8090909090909</v>
+        <v>738.8272727272727</v>
       </c>
       <c r="B92">
-        <v>1.828462867780472</v>
+        <v>0.002667249246426297</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>751.9414141414142</v>
+        <v>746.9020202020201</v>
       </c>
       <c r="B93">
-        <v>1.829586319354878</v>
+        <v>0.00264089549410671</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>760.0737373737373</v>
+        <v>754.9767676767676</v>
       </c>
       <c r="B94">
-        <v>1.830698364977078</v>
+        <v>0.002615081337935753</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>768.2060606060605</v>
+        <v>763.0515151515151</v>
       </c>
       <c r="B95">
-        <v>1.831799240642888</v>
+        <v>0.002589790133843706</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>776.3383838383838</v>
+        <v>771.1262626262626</v>
       </c>
       <c r="B96">
-        <v>1.832889175030656</v>
+        <v>0.002565005920142038</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <v>784.470707070707</v>
+        <v>779.2010101010101</v>
       </c>
       <c r="B97">
-        <v>1.833968389802072</v>
+        <v>0.002540713382762229</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>792.6030303030303</v>
+        <v>787.2757575757574</v>
       </c>
       <c r="B98">
-        <v>1.835037099887631</v>
+        <v>0.002516897822603894</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <v>800.7353535353535</v>
+        <v>795.3505050505049</v>
       </c>
       <c r="B99">
-        <v>1.836095513757688</v>
+        <v>0.002493545124844073</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
-        <v>808.8676767676767</v>
+        <v>803.4252525252524</v>
       </c>
       <c r="B100">
-        <v>1.837143833679972</v>
+        <v>0.002470641730071381</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101">
-        <v>817</v>
+        <v>811.5</v>
       </c>
       <c r="B101">
-        <v>1.838182255964352</v>
+        <v>0.002448174607119392</v>
       </c>
     </row>
   </sheetData>
@@ -2623,13 +2698,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2651,258 +2726,294 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
-        <v>11.9</v>
+        <v>62</v>
       </c>
       <c r="B2">
-        <v>1.345362404707371</v>
+        <v>12.1</v>
       </c>
       <c r="C2">
-        <v>0.151628</v>
+        <v>1.12989675044522</v>
       </c>
       <c r="D2">
-        <v>0.0243383158734444</v>
+        <v>0.113967</v>
       </c>
       <c r="E2">
-        <v>1.075546961392531</v>
+        <v>0.0111726845525644</v>
       </c>
       <c r="F2">
-        <v>-0.8192205934094156</v>
+        <v>1.08278537031645</v>
       </c>
       <c r="G2">
-        <v>-0.8512471913668236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>-0.9432208836866045</v>
+      </c>
+      <c r="H2">
+        <v>-0.928579184308906</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
-        <v>37.7</v>
+        <v>125</v>
       </c>
       <c r="B3">
-        <v>1.633333333333333</v>
+        <v>39.5</v>
       </c>
       <c r="C3">
-        <v>0.04234300000000001</v>
+        <v>1.796601730428249</v>
       </c>
       <c r="D3">
-        <v>0.002718226157707347</v>
+        <v>0.039636</v>
       </c>
       <c r="E3">
-        <v>1.576341350205793</v>
+        <v>0.002826119915675514</v>
       </c>
       <c r="F3">
-        <v>-1.373218375478392</v>
+        <v>1.59659709562646</v>
       </c>
       <c r="G3">
-        <v>-1.345009754014564</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>-1.401910180260961</v>
+      </c>
+      <c r="H3">
+        <v>-1.410745692789158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
-        <v>78.8</v>
+        <v>188</v>
       </c>
       <c r="B4">
-        <v>2.731706833139716</v>
+        <v>80.09999999999999</v>
       </c>
       <c r="C4">
-        <v>0.01997</v>
+        <v>3.572891763761611</v>
       </c>
       <c r="D4">
-        <v>0.001502090395267727</v>
+        <v>0.019578</v>
       </c>
       <c r="E4">
-        <v>1.896526217489555</v>
+        <v>0.001783419810987369</v>
       </c>
       <c r="F4">
-        <v>-1.699621935129297</v>
+        <v>1.903632516084238</v>
       </c>
       <c r="G4">
-        <v>-1.660698795510611</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>-1.708231675828481</v>
+      </c>
+      <c r="H4">
+        <v>-1.698871069010518</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
-        <v>125.4</v>
+        <v>251</v>
       </c>
       <c r="B5">
-        <v>1.528979325490629</v>
+        <v>137.2</v>
       </c>
       <c r="C5">
-        <v>0.01427</v>
+        <v>4.304519588628781</v>
       </c>
       <c r="D5">
-        <v>0.0005527145134093487</v>
+        <v>0.012534</v>
       </c>
       <c r="E5">
-        <v>2.098297536494698</v>
+        <v>0.0009046155721262668</v>
       </c>
       <c r="F5">
-        <v>-1.845576026885353</v>
+        <v>2.137354111370733</v>
       </c>
       <c r="G5">
-        <v>-1.859636974065049</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>-1.901910309636048</v>
+      </c>
+      <c r="H5">
+        <v>-1.918197954724794</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
-        <v>204.4</v>
+        <v>314</v>
       </c>
       <c r="B6">
-        <v>4.13440846232364</v>
+        <v>203.4</v>
       </c>
       <c r="C6">
-        <v>0.008930999999999998</v>
+        <v>4.77772609791171</v>
       </c>
       <c r="D6">
-        <v>0.0004717966840823608</v>
+        <v>0.008934000000000001</v>
       </c>
       <c r="E6">
-        <v>2.310480891462675</v>
+        <v>0.000431483745026649</v>
       </c>
       <c r="F6">
-        <v>-2.049099910633613</v>
+        <v>2.308350948586726</v>
       </c>
       <c r="G6">
-        <v>-2.068840989606146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>-2.04895405186418</v>
+      </c>
+      <c r="H6">
+        <v>-2.07866324560903</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
-        <v>290.6</v>
+        <v>376</v>
       </c>
       <c r="B7">
-        <v>4.487513540679045</v>
+        <v>290.4</v>
       </c>
       <c r="C7">
-        <v>0.005509</v>
+        <v>4.742713709821976</v>
       </c>
       <c r="D7">
-        <v>0.000255370971986507</v>
+        <v>0.005514</v>
       </c>
       <c r="E7">
-        <v>2.463295609962003</v>
+        <v>0.0003042593922589372</v>
       </c>
       <c r="F7">
-        <v>-2.258927227626679</v>
+        <v>2.462996612028056</v>
       </c>
       <c r="G7">
-        <v>-2.219509984111707</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>-2.258533238230245</v>
+      </c>
+      <c r="H7">
+        <v>-2.22378441727581</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
-        <v>389.3</v>
+        <v>439</v>
       </c>
       <c r="B8">
-        <v>4.887739763939974</v>
+        <v>397.9</v>
       </c>
       <c r="C8">
-        <v>0.004415000000000001</v>
+        <v>4.958606435055898</v>
       </c>
       <c r="D8">
-        <v>0.0002594791792118289</v>
+        <v>0.004329999999999999</v>
       </c>
       <c r="E8">
-        <v>2.590284403718162</v>
+        <v>0.0001732114956410868</v>
       </c>
       <c r="F8">
-        <v>-2.355069292086413</v>
+        <v>2.599773939146388</v>
       </c>
       <c r="G8">
-        <v>-2.344715684561292</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>-2.363512103646635</v>
+      </c>
+      <c r="H8">
+        <v>-2.352137747897287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
-        <v>518.1</v>
+        <v>502</v>
       </c>
       <c r="B9">
-        <v>6.563281699475246</v>
+        <v>515.9</v>
       </c>
       <c r="C9">
-        <v>0.003158</v>
+        <v>5.700779673771728</v>
       </c>
       <c r="D9">
-        <v>0.000145707469495104</v>
+        <v>0.003257</v>
       </c>
       <c r="E9">
-        <v>2.714413592287121</v>
+        <v>0.0001395711686241507</v>
       </c>
       <c r="F9">
-        <v>-2.500587874327724</v>
+        <v>2.712565527873308</v>
       </c>
       <c r="G9">
-        <v>-2.467101932523124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>-2.487182241435127</v>
+      </c>
+      <c r="H9">
+        <v>-2.457982600872541</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
-        <v>658.6</v>
+        <v>565</v>
       </c>
       <c r="B10">
-        <v>9.318082778483278</v>
+        <v>667</v>
       </c>
       <c r="C10">
-        <v>0.002616</v>
+        <v>4.695151163109069</v>
       </c>
       <c r="D10">
-        <v>0.0001107068200247843</v>
+        <v>0.002504999999999999</v>
       </c>
       <c r="E10">
-        <v>2.818621726375889</v>
+        <v>7.528095524249295E-05</v>
       </c>
       <c r="F10">
-        <v>-2.58236226034777</v>
+        <v>2.824125833916549</v>
       </c>
       <c r="G10">
-        <v>-2.569846844378747</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>-2.601192269796736</v>
+      </c>
+      <c r="H10">
+        <v>-2.56267200479263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
-        <v>817</v>
+        <v>628</v>
       </c>
       <c r="B11">
-        <v>8.299933065325822</v>
+        <v>811.5</v>
       </c>
       <c r="C11">
-        <v>0.002112</v>
+        <v>8.364275886836296</v>
       </c>
       <c r="D11">
-        <v>6.451184215148237E-05</v>
+        <v>0.002171</v>
       </c>
       <c r="E11">
-        <v>2.912222056532416</v>
+        <v>6.04510821518799E-05</v>
       </c>
       <c r="F11">
-        <v>-2.675306086138225</v>
+        <v>2.909288524162251</v>
       </c>
       <c r="G11">
-        <v>-2.662132900123662</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>-2.66334017654558</v>
+      </c>
+      <c r="H11">
+        <v>-2.642589599089996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
+        <v>638</v>
+      </c>
+      <c r="B12">
         <v>496</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.004589999999999999</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>2.891205793294678E-19</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>2.695481676490198</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>-2.338187314462739</v>
       </c>
-      <c r="G12">
-        <v>-2.448435846263907</v>
+      <c r="H12">
+        <v>-2.441950929022662</v>
       </c>
     </row>
   </sheetData>
@@ -2920,810 +3031,810 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>11.9</v>
+        <v>12.1</v>
       </c>
       <c r="B2">
-        <v>0.1512261455788152</v>
+        <v>0.114118894657337</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>20.03232323232323</v>
+        <v>20.17474747474747</v>
       </c>
       <c r="B3">
-        <v>0.08707241536200769</v>
+        <v>0.07153840198621657</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>28.16464646464647</v>
+        <v>28.24949494949495</v>
       </c>
       <c r="B4">
-        <v>0.06067855073054387</v>
+        <v>0.05259964516128546</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>36.2969696969697</v>
+        <v>36.32424242424242</v>
       </c>
       <c r="B5">
-        <v>0.04637283173295762</v>
+        <v>0.04180625295572488</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>44.42929292929293</v>
+        <v>44.3989898989899</v>
       </c>
       <c r="B6">
-        <v>0.0374283071771774</v>
+        <v>0.03480208572938091</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>52.56161616161616</v>
+        <v>52.47373737373737</v>
       </c>
       <c r="B7">
-        <v>0.03132015220138892</v>
+        <v>0.02987537705570119</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>60.6939393939394</v>
+        <v>60.54848484848484</v>
       </c>
       <c r="B8">
-        <v>0.02689064206542731</v>
+        <v>0.02621373526820083</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>68.82626262626263</v>
+        <v>68.62323232323232</v>
       </c>
       <c r="B9">
-        <v>0.02353520488954543</v>
+        <v>0.02338103360402072</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>76.95858585858586</v>
+        <v>76.69797979797978</v>
       </c>
       <c r="B10">
-        <v>0.02090772965790534</v>
+        <v>0.02112174936903392</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>85.09090909090909</v>
+        <v>84.77272727272725</v>
       </c>
       <c r="B11">
-        <v>0.01879598053660206</v>
+        <v>0.01927604335909764</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>93.22323232323232</v>
+        <v>92.84747474747473</v>
       </c>
       <c r="B12">
-        <v>0.01706267557283618</v>
+        <v>0.01773870091217781</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>101.3555555555556</v>
+        <v>100.9222222222222</v>
       </c>
       <c r="B13">
-        <v>0.01561513681367633</v>
+        <v>0.01643757540808223</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>109.4878787878788</v>
+        <v>108.9969696969697</v>
       </c>
       <c r="B14">
-        <v>0.01438856735038244</v>
+        <v>0.01532150915408134</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>117.620202020202</v>
+        <v>117.0717171717172</v>
       </c>
       <c r="B15">
-        <v>0.01333631908322386</v>
+        <v>0.01435319723341663</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>125.7525252525253</v>
+        <v>125.1464646464646</v>
       </c>
       <c r="B16">
-        <v>0.01242396639390322</v>
+        <v>0.0135047825124472</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>133.8848484848485</v>
+        <v>133.2212121212121</v>
       </c>
       <c r="B17">
-        <v>0.0116255569178896</v>
+        <v>0.01275503402534345</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>142.0171717171717</v>
+        <v>141.2959595959596</v>
       </c>
       <c r="B18">
-        <v>0.01092116092753925</v>
+        <v>0.01208748145851442</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>150.149494949495</v>
+        <v>149.3707070707071</v>
       </c>
       <c r="B19">
-        <v>0.0102952236440969</v>
+        <v>0.01148914749613198</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>158.2818181818182</v>
+        <v>157.4454545454545</v>
       </c>
       <c r="B20">
-        <v>0.009735429716742627</v>
+        <v>0.01094966553484734</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>166.4141414141414</v>
+        <v>165.520202020202</v>
       </c>
       <c r="B21">
-        <v>0.009231903447200695</v>
+        <v>0.01046065249826879</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>174.5464646464646</v>
+        <v>173.5949494949495</v>
       </c>
       <c r="B22">
-        <v>0.008776634488218677</v>
+        <v>0.01001525453838841</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>182.6787878787879</v>
+        <v>181.6696969696969</v>
       </c>
       <c r="B23">
-        <v>0.008363058253235566</v>
+        <v>0.009607812388484292</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>190.8111111111111</v>
+        <v>189.7444444444444</v>
       </c>
       <c r="B24">
-        <v>0.007985744549041576</v>
+        <v>0.009233611095551531</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>198.9434343434343</v>
+        <v>197.8191919191919</v>
       </c>
       <c r="B25">
-        <v>0.007640163239624202</v>
+        <v>0.008888690275485224</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>207.0757575757576</v>
+        <v>205.8939393939393</v>
       </c>
       <c r="B26">
-        <v>0.00732250561017831</v>
+        <v>0.00856969845168928</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>215.2080808080808</v>
+        <v>213.9686868686868</v>
       </c>
       <c r="B27">
-        <v>0.007029546589224229</v>
+        <v>0.008273779955781664</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>223.3404040404041</v>
+        <v>222.0434343434343</v>
       </c>
       <c r="B28">
-        <v>0.006758537337583468</v>
+        <v>0.007998486190224757</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>231.4727272727273</v>
+        <v>230.1181818181818</v>
       </c>
       <c r="B29">
-        <v>0.006507120680451912</v>
+        <v>0.007741705333417221</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>239.6050505050505</v>
+        <v>238.1929292929293</v>
       </c>
       <c r="B30">
-        <v>0.006273263914788072</v>
+        <v>0.007501606158254927</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>247.7373737373737</v>
+        <v>246.2676767676767</v>
       </c>
       <c r="B31">
-        <v>0.006055204969392477</v>
+        <v>0.007276592760105602</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>255.869696969697</v>
+        <v>254.3424242424242</v>
       </c>
       <c r="B32">
-        <v>0.0058514089244955</v>
+        <v>0.007065267796277352</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>264.0020202020202</v>
+        <v>262.4171717171717</v>
       </c>
       <c r="B33">
-        <v>0.005660532640093624</v>
+        <v>0.006866402423782412</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>272.1343434343434</v>
+        <v>270.4919191919192</v>
       </c>
       <c r="B34">
-        <v>0.005481395783881224</v>
+        <v>0.006678911551119365</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>280.2666666666667</v>
+        <v>278.5666666666667</v>
       </c>
       <c r="B35">
-        <v>0.005312956948981307</v>
+        <v>0.006501833337750171</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>288.3989898989899</v>
+        <v>286.6414141414141</v>
       </c>
       <c r="B36">
-        <v>0.00515429384910049</v>
+        <v>0.006334312112962199</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>296.5313131313131</v>
+        <v>294.7161616161616</v>
       </c>
       <c r="B37">
-        <v>0.005004586802319537</v>
+        <v>0.006175584065620148</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>304.6636363636363</v>
+        <v>302.7909090909091</v>
       </c>
       <c r="B38">
-        <v>0.004863104884291152</v>
+        <v>0.006024965193333106</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>312.7959595959596</v>
+        <v>310.8656565656565</v>
       </c>
       <c r="B39">
-        <v>0.004729194261270134</v>
+        <v>0.005881841104820782</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>320.9282828282828</v>
+        <v>318.940404040404</v>
       </c>
       <c r="B40">
-        <v>0.004602268313312335</v>
+        <v>0.005745658350741072</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>329.060606060606</v>
+        <v>327.0151515151515</v>
       </c>
       <c r="B41">
-        <v>0.004481799235536794</v>
+        <v>0.005615917021766245</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>337.1929292929293</v>
+        <v>335.089898989899</v>
       </c>
       <c r="B42">
-        <v>0.004367310865969389</v>
+        <v>0.005492164402560705</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>345.3252525252525</v>
+        <v>343.1646464646465</v>
       </c>
       <c r="B43">
-        <v>0.004258372536185058</v>
+        <v>0.005373989509709177</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>353.4575757575757</v>
+        <v>351.2393939393939</v>
       </c>
       <c r="B44">
-        <v>0.004154593778728686</v>
+        <v>0.005261018372958773</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>361.589898989899</v>
+        <v>359.3141414141414</v>
       </c>
       <c r="B45">
-        <v>0.004055619755368546</v>
+        <v>0.005152909944174143</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>369.7222222222222</v>
+        <v>367.3888888888889</v>
       </c>
       <c r="B46">
-        <v>0.003961127294320894</v>
+        <v>0.005049352538531013</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>377.8545454545454</v>
+        <v>375.4636363636363</v>
       </c>
       <c r="B47">
-        <v>0.003870821443975885</v>
+        <v>0.004950060728737752</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>385.9868686868687</v>
+        <v>383.5383838383838</v>
       </c>
       <c r="B48">
-        <v>0.003784432466347486</v>
+        <v>0.004854772626283929</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>394.1191919191919</v>
+        <v>391.6131313131313</v>
       </c>
       <c r="B49">
-        <v>0.003701713206230728</v>
+        <v>0.004763247494494139</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>402.2515151515152</v>
+        <v>399.6878787878787</v>
       </c>
       <c r="B50">
-        <v>0.003622436782474554</v>
+        <v>0.004675263647001852</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>410.3838383838383</v>
+        <v>407.7626262626262</v>
       </c>
       <c r="B51">
-        <v>0.003546394556332881</v>
+        <v>0.004590616592533375</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>418.5161616161616</v>
+        <v>415.8373737373737</v>
       </c>
       <c r="B52">
-        <v>0.003473394338905845</v>
+        <v>0.004509117392907075</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
-        <v>426.6484848484848</v>
+        <v>423.9121212121212</v>
       </c>
       <c r="B53">
-        <v>0.003403258805515847</v>
+        <v>0.004430591206145848</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54">
-        <v>434.7808080808081</v>
+        <v>431.9868686868687</v>
       </c>
       <c r="B54">
-        <v>0.003335824089707885</v>
+        <v>0.004354875990761184</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55">
-        <v>442.9131313131313</v>
+        <v>440.0616161616161</v>
       </c>
       <c r="B55">
-        <v>0.003270938533603003</v>
+        <v>0.004281821350746441</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56">
-        <v>451.0454545454545</v>
+        <v>448.1363636363636</v>
       </c>
       <c r="B56">
-        <v>0.003208461574713612</v>
+        <v>0.004211287503737038</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <v>459.1777777777777</v>
+        <v>456.2111111111111</v>
       </c>
       <c r="B57">
-        <v>0.003148262752167272</v>
+        <v>0.00414314435725427</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <v>467.310101010101</v>
+        <v>464.2858585858585</v>
       </c>
       <c r="B58">
-        <v>0.00309022081767621</v>
+        <v>0.00407727068002698</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <v>475.4424242424242</v>
+        <v>472.360606060606</v>
       </c>
       <c r="B59">
-        <v>0.003034222938610254</v>
+        <v>0.004013553357146009</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <v>483.5747474747474</v>
+        <v>480.4353535353535</v>
       </c>
       <c r="B60">
-        <v>0.002980163982243562</v>
+        <v>0.003951886719303136</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <v>491.7070707070707</v>
+        <v>488.510101010101</v>
       </c>
       <c r="B61">
-        <v>0.002927945871701747</v>
+        <v>0.003892171937642248</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>499.8393939393939</v>
+        <v>496.5848484848485</v>
       </c>
       <c r="B62">
-        <v>0.002877477005377666</v>
+        <v>0.003834316476841483</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>507.9717171717172</v>
+        <v>504.6595959595959</v>
       </c>
       <c r="B63">
-        <v>0.002828671732645802</v>
+        <v>0.003778233599980349</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>516.1040404040403</v>
+        <v>512.7343434343434</v>
       </c>
       <c r="B64">
-        <v>0.002781449879615335</v>
+        <v>0.003723841919549707</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>524.2363636363636</v>
+        <v>520.8090909090909</v>
       </c>
       <c r="B65">
-        <v>0.002735736319444319</v>
+        <v>0.003671064989655256</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>532.3686868686868</v>
+        <v>528.8838383838383</v>
       </c>
       <c r="B66">
-        <v>0.002691460582411479</v>
+        <v>0.003619830935063521</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>540.50101010101</v>
+        <v>536.9585858585858</v>
       </c>
       <c r="B67">
-        <v>0.002648556501524354</v>
+        <v>0.003570072113257467</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>548.6333333333333</v>
+        <v>545.0333333333333</v>
       </c>
       <c r="B68">
-        <v>0.002606961889946678</v>
+        <v>0.003521724806118537</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>556.7656565656565</v>
+        <v>553.1080808080808</v>
       </c>
       <c r="B69">
-        <v>0.002566618246965211</v>
+        <v>0.003474728938243024</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>564.8979797979798</v>
+        <v>561.1828282828283</v>
       </c>
       <c r="B70">
-        <v>0.002527470489596689</v>
+        <v>0.003429027819241569</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>573.030303030303</v>
+        <v>569.2575757575758</v>
       </c>
       <c r="B71">
-        <v>0.002489466707267035</v>
+        <v>0.003384567907668399</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>581.1626262626262</v>
+        <v>577.3323232323232</v>
       </c>
       <c r="B72">
-        <v>0.002452557937284456</v>
+        <v>0.003341298594487549</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>589.2949494949495</v>
+        <v>585.4070707070706</v>
       </c>
       <c r="B73">
-        <v>0.002416697959081371</v>
+        <v>0.00329917200421184</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>597.4272727272727</v>
+        <v>593.4818181818181</v>
       </c>
       <c r="B74">
-        <v>0.002381843105422225</v>
+        <v>0.003258142812051314</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>605.559595959596</v>
+        <v>601.5565656565656</v>
       </c>
       <c r="B75">
-        <v>0.002347952088969245</v>
+        <v>0.003218168075584502</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>613.6919191919192</v>
+        <v>609.631313131313</v>
       </c>
       <c r="B76">
-        <v>0.00231498584276996</v>
+        <v>0.003179207079621927</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>621.8242424242424</v>
+        <v>617.7060606060605</v>
       </c>
       <c r="B77">
-        <v>0.002282907373381544</v>
+        <v>0.003141221193068869</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>629.9565656565657</v>
+        <v>625.780808080808</v>
       </c>
       <c r="B78">
-        <v>0.00225168162548074</v>
+        <v>0.003104173736716384</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>638.0888888888888</v>
+        <v>633.8555555555555</v>
       </c>
       <c r="B79">
-        <v>0.002221275356926324</v>
+        <v>0.003068029860997553</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>646.221212121212</v>
+        <v>641.930303030303</v>
       </c>
       <c r="B80">
-        <v>0.002191657023345785</v>
+        <v>0.003032756432841862</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <v>654.3535353535353</v>
+        <v>650.0050505050505</v>
       </c>
       <c r="B81">
-        <v>0.002162796671410889</v>
+        <v>0.002998321930845916</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82">
-        <v>662.4858585858585</v>
+        <v>658.0797979797979</v>
       </c>
       <c r="B82">
-        <v>0.002134665840049385</v>
+        <v>0.002964696348054624</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <v>670.6181818181818</v>
+        <v>666.1545454545454</v>
       </c>
       <c r="B83">
-        <v>0.002107237468913657</v>
+        <v>0.002931851101714743</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <v>678.750505050505</v>
+        <v>674.2292929292929</v>
       </c>
       <c r="B84">
-        <v>0.002080485813492712</v>
+        <v>0.002899758949423204</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>686.8828282828282</v>
+        <v>682.3040404040404</v>
       </c>
       <c r="B85">
-        <v>0.002054386366312409</v>
+        <v>0.002868393911146696</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <v>695.0151515151515</v>
+        <v>690.3787878787878</v>
       </c>
       <c r="B86">
-        <v>0.002028915783721162</v>
+        <v>0.002837731196637552</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <v>703.1474747474747</v>
+        <v>698.4535353535352</v>
       </c>
       <c r="B87">
-        <v>0.00200405181780522</v>
+        <v>0.002807747137814382</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <v>711.279797979798</v>
+        <v>706.5282828282827</v>
       </c>
       <c r="B88">
-        <v>0.001979773253019607</v>
+        <v>0.002778419125714995</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>719.4121212121212</v>
+        <v>714.6030303030302</v>
       </c>
       <c r="B89">
-        <v>0.001956059847158515</v>
+        <v>0.002749725551664224</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <v>727.5444444444444</v>
+        <v>722.6777777777777</v>
       </c>
       <c r="B90">
-        <v>0.001932892276322811</v>
+        <v>0.002721645752330935</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>735.6767676767677</v>
+        <v>730.7525252525252</v>
       </c>
       <c r="B91">
-        <v>0.001910252083572831</v>
+        <v>0.00269415995837694</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
-        <v>743.8090909090909</v>
+        <v>738.8272727272727</v>
       </c>
       <c r="B92">
-        <v>0.001888121630982088</v>
+        <v>0.002667249246426297</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>751.9414141414142</v>
+        <v>746.9020202020201</v>
       </c>
       <c r="B93">
-        <v>0.001866484054832298</v>
+        <v>0.00264089549410671</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>760.0737373737373</v>
+        <v>754.9767676767676</v>
       </c>
       <c r="B94">
-        <v>0.001845323223712523</v>
+        <v>0.002615081337935753</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>768.2060606060605</v>
+        <v>763.0515151515151</v>
       </c>
       <c r="B95">
-        <v>0.001824623699305458</v>
+        <v>0.002589790133843706</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>776.3383838383838</v>
+        <v>771.1262626262626</v>
       </c>
       <c r="B96">
-        <v>0.001804370699662181</v>
+        <v>0.002565005920142038</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <v>784.470707070707</v>
+        <v>779.2010101010101</v>
       </c>
       <c r="B97">
-        <v>0.00178455006478332</v>
+        <v>0.002540713382762229</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>792.6030303030303</v>
+        <v>787.2757575757574</v>
       </c>
       <c r="B98">
-        <v>0.0017651482243396</v>
+        <v>0.002516897822603894</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <v>800.7353535353535</v>
+        <v>795.3505050505049</v>
       </c>
       <c r="B99">
-        <v>0.001746152167378434</v>
+        <v>0.002493545124844073</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
-        <v>808.8676767676767</v>
+        <v>803.4252525252524</v>
       </c>
       <c r="B100">
-        <v>0.00172754941387562</v>
+        <v>0.002470641730071381</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101">
-        <v>817</v>
+        <v>811.5</v>
       </c>
       <c r="B101">
-        <v>0.001709327988002532</v>
+        <v>0.002448174607119392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>